<commit_message>
Rearranged SmartSession: take the desired prototype bases as your initial launch base.
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Goal" sheetId="2" r:id="rId1"/>
     <sheet name="GoalTask" sheetId="1" r:id="rId2"/>
+    <sheet name="Video" sheetId="3" r:id="rId3"/>
+    <sheet name="MusicFile" sheetId="4" r:id="rId4"/>
+    <sheet name="Book" sheetId="5" r:id="rId5"/>
+    <sheet name="Hyperlink" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -60,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>GoalTaskType</t>
   </si>
@@ -83,10 +87,34 @@
     <t>2012-03-22 10:32:10</t>
   </si>
   <si>
-    <t>Task Title</t>
-  </si>
-  <si>
-    <t>Notes for this task.</t>
+    <t>Finger Independence Exercises: Examples 1a to 2b</t>
+  </si>
+  <si>
+    <t>Finger Independence Exercises: Examples 2c to 3g</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Strength,Independence,Dexterity</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Source Type</t>
+  </si>
+  <si>
+    <t>Kindle Book</t>
+  </si>
+  <si>
+    <t>Complete Technique for Modern Guitar</t>
+  </si>
+  <si>
+    <t>Video File</t>
+  </si>
+  <si>
+    <t>Hal Leonard - Classic Metal - Volume 8</t>
   </si>
 </sst>
 </file>
@@ -445,7 +473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -455,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,11 +496,14 @@
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="8" max="8" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,10 +517,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -501,26 +543,41 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -528,7 +585,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -536,7 +593,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -544,7 +601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -552,7 +609,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -560,7 +617,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -568,7 +625,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -576,7 +633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -584,7 +641,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -592,7 +649,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -600,7 +657,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -608,7 +665,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -725,4 +782,58 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>